<commit_message>
avace SP ROL pt 1
</commit_message>
<xml_diff>
--- a/DB-DOCs/PROCEDIMIENTOS LOAsi.xlsx
+++ b/DB-DOCs/PROCEDIMIENTOS LOAsi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhose\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REPOSITORIOS GIT FORK\NODEJS\web_api_store\DB-DOCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF7E1EB-DA3B-485F-BB5E-CE5A76AE7C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06E943F-7E4F-4E68-B2A8-5A3E9A4A6014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25050" yWindow="3180" windowWidth="20910" windowHeight="11835" xr2:uid="{AC2CF57E-2B11-4527-92FD-CE7DEF6D8F3E}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="20910" windowHeight="11835" xr2:uid="{AC2CF57E-2B11-4527-92FD-CE7DEF6D8F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="33">
   <si>
     <t>ProductsByCategoryANDORActive</t>
   </si>
@@ -125,20 +125,20 @@
     <t>YA</t>
   </si>
   <si>
-    <t>getAllretiros</t>
-  </si>
-  <si>
     <t>VER DESDE AHI POSTMAN</t>
   </si>
   <si>
     <t>EMPLOYEE reservado para hacer testeos</t>
+  </si>
+  <si>
+    <t>getAllRetiros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +163,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -173,12 +179,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -186,24 +192,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,340 +544,354 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA357EB-89F5-4754-8972-1AC3BCF685D1}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>